<commit_message>
New scenarios with dialogue and module descriptions also in English
</commit_message>
<xml_diff>
--- a/Assets/Resources/Localization/SUGARUnityLocalization.xlsx
+++ b/Assets/Resources/Localization/SUGARUnityLocalization.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Documents\Projects\RAGE\SpaceMods\Assets\Resources\Localization\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="510" yWindow="600" windowWidth="24620" windowHeight="11960"/>
+    <workbookView xWindow="510" yWindow="600" windowWidth="24615" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="SUGARLocalizations" sheetId="1" r:id="rId1"/>
@@ -24,9 +19,6 @@
     <t>Key</t>
   </si>
   <si>
-    <t>en-gb</t>
-  </si>
-  <si>
     <t>ACHIEVEMENT_LOAD_ERROR</t>
   </si>
   <si>
@@ -374,6 +366,9 @@
   </si>
   <si>
     <t>Fout: Kan geen lijst met groepsleden krijgen</t>
+  </si>
+  <si>
+    <t>en</t>
   </si>
 </sst>
 </file>
@@ -497,7 +492,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -532,7 +527,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -747,466 +742,466 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C46" sqref="C46"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.7265625" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" customWidth="1"/>
     <col min="2" max="2" width="58" customWidth="1"/>
-    <col min="3" max="3" width="54.81640625" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="C39" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C40" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>